<commit_message>
Corrected data point. For fish_id f0001 (dob '20201014'), corrected age from '10month' to '13month'.
</commit_message>
<xml_diff>
--- a/figure_1A_1B/summary_weight_length_data_jag2b_6wpf_to_2yrold_20230303bld.xlsx
+++ b/figure_1A_1B/summary_weight_length_data_jag2b_6wpf_to_2yrold_20230303bld.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bdemarest/work/lalmero/jag2b_manuscript_figures/figure_1A_1B/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23B77C2-CE5F-754A-B602-7D38AD1502C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B88B54-78B8-E54E-87D0-D35DE9C6DCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1120" windowWidth="19820" windowHeight="25160" xr2:uid="{395F6B9D-67B0-0C49-BBB1-354C592C1F18}"/>
+    <workbookView xWindow="1620" yWindow="1660" windowWidth="19820" windowHeight="24360" xr2:uid="{395F6B9D-67B0-0C49-BBB1-354C592C1F18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1247,8 +1247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8B0ABE-F848-7545-ACC4-9CE54AD78359}">
   <dimension ref="A1:H259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C251" sqref="C251"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F211" sqref="F211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6381,7 +6382,7 @@
         <v>3.5840000000000001</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G211" s="1">
         <v>20201014</v>

</xml_diff>